<commit_message>
Change in excel data and code
</commit_message>
<xml_diff>
--- a/src/main/resources/Scenarios/keywordDriven.xlsx
+++ b/src/main/resources/Scenarios/keywordDriven.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ntlgnoida-my.sharepoint.com/personal/ashutosh_1_k_coforge_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDFE0BAE-3B63-4EB3-9B5F-A6E3EA863136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{CDFE0BAE-3B63-4EB3-9B5F-A6E3EA863136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{006F6014-3906-4FA1-8BD5-04FF066EC19E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{222BC742-D9E3-452A-BFF0-BFB63F819B13}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Test Step</t>
   </si>
   <si>
-    <t>Locator</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>https://opensource-demo.orangehrmlive.com/</t>
   </si>
   <si>
-    <t>id=txtUsername</t>
-  </si>
-  <si>
     <t>sendkeys</t>
   </si>
   <si>
@@ -78,18 +72,12 @@
     <t>enter password</t>
   </si>
   <si>
-    <t>id=txtPassword</t>
-  </si>
-  <si>
     <t>admin123</t>
   </si>
   <si>
     <t>click on login button</t>
   </si>
   <si>
-    <t>id=btnLogin</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -97,6 +85,24 @@
   </si>
   <si>
     <t>quit</t>
+  </si>
+  <si>
+    <t>Locator value</t>
+  </si>
+  <si>
+    <t>txtUsername</t>
+  </si>
+  <si>
+    <t>txtPassword</t>
+  </si>
+  <si>
+    <t>btnLogin</t>
+  </si>
+  <si>
+    <t>Locator Name</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -474,121 +480,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE226DE-A308-4459-A99B-5FCAF698E4DE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="40.1796875" customWidth="1"/>
+    <col min="2" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="40.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
+      <c r="E7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{DF8E8A09-DAE8-44B5-822E-2B44C3749F15}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{DF8E8A09-DAE8-44B5-822E-2B44C3749F15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>